<commit_message>
Added scripts for AUDNZD pair
</commit_message>
<xml_diff>
--- a/AlgoDB/insertFromMT.xlsx
+++ b/AlgoDB/insertFromMT.xlsx
@@ -19,7 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>EURUSD_H1</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -501,9 +505,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -825,23 +830,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="G1:R100014"/>
+  <dimension ref="G1:S100014"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="17:18" x14ac:dyDescent="0.25">
-      <c r="Q1" t="str">
-        <f>"insert into EURUSD_H1(newdatetime, open,high,low,close,volume,macd,cci,atr,bollh,bollm,bolll,dema,ma,mom) values(to_date('"&amp;A1&amp;"','YYYY.MM.DD.HH24:MI'), "&amp;B1&amp;","&amp;C1&amp;","&amp;D1&amp;","&amp;E1&amp;","&amp;F1&amp;","&amp;G1&amp;","&amp;H1&amp;","&amp;I1&amp;","&amp;J1&amp;","&amp;K1&amp;","&amp;L1&amp;","&amp;M1&amp;","&amp;N1&amp;","&amp;O1&amp;");"</f>
+    <row r="1" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" t="str">
+        <f>"insert into "&amp;$Q$1&amp;"(newdatetime, open,high,low,close,volume,macd,cci,atr,bollh,bollm,bolll,dema,ma,mom) values(to_date('"&amp;A1&amp;"','YYYY.MM.DD.HH24:MI'), "&amp;B1&amp;","&amp;C1&amp;","&amp;D1&amp;","&amp;E1&amp;","&amp;F1&amp;","&amp;G1&amp;","&amp;H1&amp;","&amp;I1&amp;","&amp;J1&amp;","&amp;K1&amp;","&amp;L1&amp;","&amp;M1&amp;","&amp;N1&amp;","&amp;O1&amp;");"</f>
         <v>insert into EURUSD_H1(newdatetime, open,high,low,close,volume,macd,cci,atr,bollh,bollm,bolll,dema,ma,mom) values(to_date('','YYYY.MM.DD.HH24:MI'), ,,,,,,,,,,,,,);</v>
       </c>
-      <c r="R1" t="str">
-        <f>"update EURUSD_H1 set MACD="&amp;G1&amp;", CCI="&amp;H1&amp;", ATR="&amp;I1&amp;", BOLLH="&amp;J1&amp;", BOLLM="&amp;K1&amp;", BOLLL="&amp;L1&amp;", DEMA="&amp;M1&amp;", MA="&amp;N1&amp;", MOM="&amp;O1&amp;" where newdatetime=to_date('"&amp;A1&amp;"','YYYY.MM.DD.HH24:MI');"</f>
-        <v>update EURUSD_H1 set MACD=, CCI=, ATR=, BOLLH=, BOLLM=, BOLLL=, DEMA=, MA=, MOM= where newdatetime=to_date('','YYYY.MM.DD.HH24:MI');</v>
+      <c r="S1" t="str">
+        <f>"update "&amp;$Q$1&amp;"EURUSD_H1 set MACD="&amp;G1&amp;", CCI="&amp;H1&amp;", ATR="&amp;I1&amp;", BOLLH="&amp;J1&amp;", BOLLM="&amp;K1&amp;", BOLLL="&amp;L1&amp;", DEMA="&amp;M1&amp;", MA="&amp;N1&amp;", MOM="&amp;O1&amp;" where newdatetime=to_date('"&amp;A1&amp;"','YYYY.MM.DD.HH24:MI');"</f>
+        <v>update EURUSD_H1EURUSD_H1 set MACD=, CCI=, ATR=, BOLLH=, BOLLM=, BOLLL=, DEMA=, MA=, MOM= where newdatetime=to_date('','YYYY.MM.DD.HH24:MI');</v>
       </c>
     </row>
     <row r="19" spans="7:7" x14ac:dyDescent="0.25">
@@ -37171,5 +37183,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>